<commit_message>
Update .CSV to include date hired
</commit_message>
<xml_diff>
--- a/Employee/Employee_Data.xlsx
+++ b/Employee/Employee_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fdbb21a5dbde31e1/Documents/UVic/CSC 370/Database Project/Employee/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="159" documentId="11_F25DC773A252ABDACC1048F3C95B666E5ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0D41648B-9F95-47E0-B51F-D797D1E6590C}"/>
+  <xr:revisionPtr revIDLastSave="198" documentId="11_F25DC773A252ABDACC1048F3C95B666E5ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{933F61BF-5A64-44CF-94DE-BD2FA8728B78}"/>
   <bookViews>
-    <workbookView xWindow="9420" yWindow="540" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,16 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="25">
-  <si>
-    <t>Employee_ID</t>
-  </si>
-  <si>
-    <t>Age</t>
-  </si>
-  <si>
-    <t>Name</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>"Bank Sinatra"</t>
   </si>
@@ -75,12 +66,6 @@
     <t>"Military Bank"</t>
   </si>
   <si>
-    <t>Title</t>
-  </si>
-  <si>
-    <t>Is_Admin</t>
-  </si>
-  <si>
     <t>Assistant Branch Manager</t>
   </si>
   <si>
@@ -100,12 +85,36 @@
   </si>
   <si>
     <t>Branch Manager'</t>
+  </si>
+  <si>
+    <t>employee_id</t>
+  </si>
+  <si>
+    <t>age</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>title</t>
+  </si>
+  <si>
+    <t>is_admin</t>
+  </si>
+  <si>
+    <t>branch_num</t>
+  </si>
+  <si>
+    <t>hire_date</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -135,9 +144,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -153,10 +163,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -422,10 +428,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G17" sqref="G17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -435,29 +441,37 @@
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="33.28515625" customWidth="1"/>
     <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="7" max="7" width="13.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="7" max="7" width="21" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" customWidth="1"/>
     <col min="10" max="10" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
       <c r="D1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="F1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -465,16 +479,22 @@
         <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>20240601</v>
+      </c>
+      <c r="G2" s="2">
+        <v>36682</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -482,16 +502,22 @@
         <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>20240601</v>
+      </c>
+      <c r="G3" s="2">
+        <v>36683</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -499,16 +525,22 @@
         <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="E4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>20240601</v>
+      </c>
+      <c r="G4" s="2">
+        <v>40221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -516,16 +548,22 @@
         <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>20240601</v>
+      </c>
+      <c r="G5" s="2">
+        <v>38701</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -533,16 +571,22 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>20240601</v>
+      </c>
+      <c r="G6" s="2">
+        <v>37257</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -550,16 +594,22 @@
         <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>20240601</v>
+      </c>
+      <c r="G7" s="2">
+        <v>41558</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -567,16 +617,22 @@
         <v>65</v>
       </c>
       <c r="C8" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>20240601</v>
+      </c>
+      <c r="G8" s="2">
+        <v>42179</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -584,16 +640,22 @@
         <v>77</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="E9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>20240601</v>
+      </c>
+      <c r="G9" s="2">
+        <v>39902</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -601,16 +663,22 @@
         <v>65</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>20240601</v>
+      </c>
+      <c r="G10" s="2">
+        <v>39133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -618,16 +686,22 @@
         <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="D11" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>20240601</v>
+      </c>
+      <c r="G11" s="2">
+        <v>37410</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -635,16 +709,22 @@
         <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>20240601</v>
+      </c>
+      <c r="G12" s="2">
+        <v>40442</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -652,16 +732,22 @@
         <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="D13" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>20240601</v>
+      </c>
+      <c r="G13" s="2">
+        <v>40858</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -669,16 +755,22 @@
         <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14">
+        <v>20240601</v>
+      </c>
+      <c r="G14" s="2">
+        <v>38135</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -686,16 +778,22 @@
         <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15">
+        <v>20240601</v>
+      </c>
+      <c r="G15" s="2">
+        <v>41356</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -703,13 +801,19 @@
         <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="E16">
         <v>0</v>
+      </c>
+      <c r="F16">
+        <v>20240601</v>
+      </c>
+      <c r="G16" s="2">
+        <v>38564</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Employee files, Added Position files
</commit_message>
<xml_diff>
--- a/Employee/Employee_Data.xlsx
+++ b/Employee/Employee_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fdbb21a5dbde31e1/Documents/UVic/CSC 370/Database Project/Employee/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="200" documentId="11_F25DC773A252ABDACC1048F3C95B666E5ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4778C1FF-9BBA-42C9-A93E-3412484BF280}"/>
+  <xr:revisionPtr revIDLastSave="239" documentId="11_F25DC773A252ABDACC1048F3C95B666E5ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E911CF77-CE38-4897-9029-26251C20ACA5}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
     <t>"Bank Sinatra"</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Customer Service Representative</t>
   </si>
   <si>
-    <t>Branch Manager'</t>
-  </si>
-  <si>
     <t>employee_id</t>
   </si>
   <si>
@@ -99,13 +96,13 @@
     <t>title</t>
   </si>
   <si>
-    <t>is_admin</t>
-  </si>
-  <si>
     <t>branch_num</t>
   </si>
   <si>
     <t>hire_date</t>
+  </si>
+  <si>
+    <t>Branch Manager</t>
   </si>
 </sst>
 </file>
@@ -144,10 +141,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -432,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -445,40 +443,34 @@
     <col min="3" max="3" width="16" customWidth="1"/>
     <col min="4" max="4" width="33.28515625" customWidth="1"/>
     <col min="5" max="5" width="12.140625" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
+    <col min="6" max="6" width="18.28515625" customWidth="1"/>
     <col min="7" max="7" width="21" customWidth="1"/>
     <col min="8" max="8" width="20.42578125" customWidth="1"/>
     <col min="9" max="9" width="15.7109375" customWidth="1"/>
     <col min="10" max="10" width="33.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
         <v>20</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>21</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>22</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>23</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="F1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -489,22 +481,17 @@
         <v>0</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>20240601</v>
-      </c>
-      <c r="G2" s="2">
+        <v>25</v>
+      </c>
+      <c r="E2" s="3">
+        <v>1005151</v>
+      </c>
+      <c r="F2" s="2">
         <v>36682</v>
       </c>
-      <c r="H2" s="2">
-        <v>36682</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -517,20 +504,15 @@
       <c r="D3" t="s">
         <v>13</v>
       </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>20240601</v>
-      </c>
-      <c r="G3" s="2">
+      <c r="E3" s="3">
+        <v>1005151</v>
+      </c>
+      <c r="F3" s="2">
         <v>36683</v>
       </c>
-      <c r="H3" s="2">
-        <v>36683</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G3" s="2"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -543,20 +525,15 @@
       <c r="D4" t="s">
         <v>14</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>20240601</v>
-      </c>
-      <c r="G4" s="2">
+      <c r="E4" s="3">
+        <v>1005151</v>
+      </c>
+      <c r="F4" s="2">
         <v>40221</v>
       </c>
-      <c r="H4" s="2">
-        <v>40221</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -569,20 +546,15 @@
       <c r="D5" t="s">
         <v>15</v>
       </c>
-      <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>20240601</v>
-      </c>
-      <c r="G5" s="2">
+      <c r="E5" s="3">
+        <v>1005151</v>
+      </c>
+      <c r="F5" s="2">
         <v>38701</v>
       </c>
-      <c r="H5" s="2">
-        <v>38701</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G5" s="2"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -595,20 +567,15 @@
       <c r="D6" t="s">
         <v>15</v>
       </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6">
-        <v>20240601</v>
-      </c>
-      <c r="G6" s="2">
+      <c r="E6" s="3">
+        <v>1005151</v>
+      </c>
+      <c r="F6" s="2">
         <v>37257</v>
       </c>
-      <c r="H6" s="2">
-        <v>37257</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G6" s="2"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -621,20 +588,15 @@
       <c r="D7" t="s">
         <v>15</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7">
-        <v>20240601</v>
-      </c>
-      <c r="G7" s="2">
+      <c r="E7" s="3">
+        <v>1005151</v>
+      </c>
+      <c r="F7" s="2">
         <v>41558</v>
       </c>
-      <c r="H7" s="2">
-        <v>41558</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G7" s="2"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -647,20 +609,15 @@
       <c r="D8" t="s">
         <v>15</v>
       </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8">
-        <v>20240601</v>
-      </c>
-      <c r="G8" s="2">
+      <c r="E8" s="3">
+        <v>1005151</v>
+      </c>
+      <c r="F8" s="2">
         <v>42179</v>
       </c>
-      <c r="H8" s="2">
-        <v>42179</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G8" s="2"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -673,20 +630,15 @@
       <c r="D9" t="s">
         <v>15</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9">
-        <v>20240601</v>
-      </c>
-      <c r="G9" s="2">
+      <c r="E9" s="3">
+        <v>1005151</v>
+      </c>
+      <c r="F9" s="2">
         <v>39902</v>
       </c>
-      <c r="H9" s="2">
-        <v>39902</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G9" s="2"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -699,20 +651,15 @@
       <c r="D10" t="s">
         <v>16</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10">
-        <v>20240601</v>
-      </c>
-      <c r="G10" s="2">
+      <c r="E10" s="3">
+        <v>1005151</v>
+      </c>
+      <c r="F10" s="2">
         <v>39133</v>
       </c>
-      <c r="H10" s="2">
-        <v>39133</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G10" s="2"/>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -725,20 +672,15 @@
       <c r="D11" t="s">
         <v>16</v>
       </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11">
-        <v>20240601</v>
-      </c>
-      <c r="G11" s="2">
+      <c r="E11" s="3">
+        <v>1005151</v>
+      </c>
+      <c r="F11" s="2">
         <v>37410</v>
       </c>
-      <c r="H11" s="2">
-        <v>37410</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G11" s="2"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -751,20 +693,15 @@
       <c r="D12" t="s">
         <v>16</v>
       </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>20240601</v>
-      </c>
-      <c r="G12" s="2">
+      <c r="E12" s="3">
+        <v>1005151</v>
+      </c>
+      <c r="F12" s="2">
         <v>40442</v>
       </c>
-      <c r="H12" s="2">
-        <v>40442</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G12" s="2"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -777,20 +714,15 @@
       <c r="D13" t="s">
         <v>18</v>
       </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>20240601</v>
-      </c>
-      <c r="G13" s="2">
+      <c r="E13" s="3">
+        <v>1005151</v>
+      </c>
+      <c r="F13" s="2">
         <v>40858</v>
       </c>
-      <c r="H13" s="2">
-        <v>40858</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G13" s="2"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -803,20 +735,15 @@
       <c r="D14" t="s">
         <v>17</v>
       </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>20240601</v>
-      </c>
-      <c r="G14" s="2">
+      <c r="E14" s="3">
+        <v>1005151</v>
+      </c>
+      <c r="F14" s="2">
         <v>38135</v>
       </c>
-      <c r="H14" s="2">
-        <v>38135</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G14" s="2"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -829,20 +756,15 @@
       <c r="D15" t="s">
         <v>17</v>
       </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>20240601</v>
-      </c>
-      <c r="G15" s="2">
+      <c r="E15" s="3">
+        <v>1005151</v>
+      </c>
+      <c r="F15" s="2">
         <v>41356</v>
       </c>
-      <c r="H15" s="2">
-        <v>41356</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G15" s="2"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -855,18 +777,13 @@
       <c r="D16" t="s">
         <v>17</v>
       </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>20240601</v>
-      </c>
-      <c r="G16" s="2">
+      <c r="E16" s="3">
+        <v>1005151</v>
+      </c>
+      <c r="F16" s="2">
         <v>38564</v>
       </c>
-      <c r="H16" s="2">
-        <v>38564</v>
-      </c>
+      <c r="G16" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added more queries and data
</commit_message>
<xml_diff>
--- a/Employee/Employee_Data.xlsx
+++ b/Employee/Employee_Data.xlsx
@@ -8,63 +8,35 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fdbb21a5dbde31e1/Documents/UVic/CSC 370/Database Project/Employee/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="239" documentId="11_F25DC773A252ABDACC1048F3C95B666E5ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E911CF77-CE38-4897-9029-26251C20ACA5}"/>
+  <xr:revisionPtr revIDLastSave="321" documentId="11_F25DC773A252ABDACC1048F3C95B666E5ADE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F14773F7-E50E-4CC1-BA2B-90F7339D9DAC}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
-  <si>
-    <t>"Bank Sinatra"</t>
-  </si>
-  <si>
-    <t>"Bank Langella"</t>
-  </si>
-  <si>
-    <t>"Anne Bank"</t>
-  </si>
-  <si>
-    <t>"Bank and File"</t>
-  </si>
-  <si>
-    <t>"Draw a Bank"</t>
-  </si>
-  <si>
-    <t>"Point-Bank"</t>
-  </si>
-  <si>
-    <t>"Walk the Bank"</t>
-  </si>
-  <si>
-    <t>"Bank Zappa"</t>
-  </si>
-  <si>
-    <t>"Bank Ocean"</t>
-  </si>
-  <si>
-    <t>"Purple Bank"</t>
-  </si>
-  <si>
-    <t>"Bank You"</t>
-  </si>
-  <si>
-    <t>"Swiss Bank"</t>
-  </si>
-  <si>
-    <t>"Military Bank"</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="41">
   <si>
     <t>Assistant Branch Manager</t>
   </si>
@@ -103,6 +75,90 @@
   </si>
   <si>
     <t>Branch Manager</t>
+  </si>
+  <si>
+    <t>Bank Sinatra</t>
+  </si>
+  <si>
+    <t>Bank Langella</t>
+  </si>
+  <si>
+    <t>Anne Bank</t>
+  </si>
+  <si>
+    <t>Bank and File</t>
+  </si>
+  <si>
+    <t>Draw a Bank</t>
+  </si>
+  <si>
+    <t>Point-Bank</t>
+  </si>
+  <si>
+    <t>Walk the Bank</t>
+  </si>
+  <si>
+    <t>Bank Ocean</t>
+  </si>
+  <si>
+    <t>Bank Zappa</t>
+  </si>
+  <si>
+    <t>Purple Bank</t>
+  </si>
+  <si>
+    <t>Bank You</t>
+  </si>
+  <si>
+    <t>Swiss Bank</t>
+  </si>
+  <si>
+    <t>Military Bank</t>
+  </si>
+  <si>
+    <t>Money Man</t>
+  </si>
+  <si>
+    <t>Money Man Two</t>
+  </si>
+  <si>
+    <t>Mo Money</t>
+  </si>
+  <si>
+    <t>Money Honey</t>
+  </si>
+  <si>
+    <t>Bands of Money</t>
+  </si>
+  <si>
+    <t>Fake Money</t>
+  </si>
+  <si>
+    <t>No Money</t>
+  </si>
+  <si>
+    <t>Money Money</t>
+  </si>
+  <si>
+    <t>Money</t>
+  </si>
+  <si>
+    <t>Less Money</t>
+  </si>
+  <si>
+    <t>Money Less</t>
+  </si>
+  <si>
+    <t>Who Has Money</t>
+  </si>
+  <si>
+    <t>Out Of Money</t>
+  </si>
+  <si>
+    <t>My Money</t>
+  </si>
+  <si>
+    <t>Our Money</t>
   </si>
 </sst>
 </file>
@@ -141,11 +197,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,10 +487,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -452,22 +509,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="F1" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -478,15 +535,15 @@
         <v>32</v>
       </c>
       <c r="C2" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="E2" s="3">
         <v>1005151</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="4">
         <v>36682</v>
       </c>
       <c r="G2" s="2"/>
@@ -499,15 +556,15 @@
         <v>31</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="D3" t="s">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E3" s="3">
         <v>1005151</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="4">
         <v>36683</v>
       </c>
       <c r="G3" s="2"/>
@@ -520,15 +577,15 @@
         <v>54</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="D4" t="s">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="E4" s="3">
         <v>1005151</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="4">
         <v>40221</v>
       </c>
       <c r="G4" s="2"/>
@@ -541,15 +598,15 @@
         <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E5" s="3">
         <v>1005151</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="4">
         <v>38701</v>
       </c>
       <c r="G5" s="2"/>
@@ -562,15 +619,15 @@
         <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E6" s="3">
         <v>1005151</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="4">
         <v>37257</v>
       </c>
       <c r="G6" s="2"/>
@@ -583,15 +640,15 @@
         <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>18</v>
       </c>
       <c r="D7" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E7" s="3">
         <v>1005151</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="4">
         <v>41558</v>
       </c>
       <c r="G7" s="2"/>
@@ -604,15 +661,15 @@
         <v>65</v>
       </c>
       <c r="C8" t="s">
-        <v>6</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E8" s="3">
         <v>1005151</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="4">
         <v>42179</v>
       </c>
       <c r="G8" s="2"/>
@@ -625,15 +682,15 @@
         <v>77</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="D9" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="E9" s="3">
         <v>1005151</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="4">
         <v>39902</v>
       </c>
       <c r="G9" s="2"/>
@@ -646,15 +703,15 @@
         <v>65</v>
       </c>
       <c r="C10" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D10" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E10" s="3">
         <v>1005151</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="4">
         <v>39133</v>
       </c>
       <c r="G10" s="2"/>
@@ -667,15 +724,15 @@
         <v>54</v>
       </c>
       <c r="C11" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D11" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E11" s="3">
         <v>1005151</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="4">
         <v>37410</v>
       </c>
       <c r="G11" s="2"/>
@@ -688,15 +745,15 @@
         <v>33</v>
       </c>
       <c r="C12" t="s">
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="D12" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="E12" s="3">
         <v>1005151</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="4">
         <v>40442</v>
       </c>
       <c r="G12" s="2"/>
@@ -709,15 +766,15 @@
         <v>36</v>
       </c>
       <c r="C13" t="s">
-        <v>9</v>
+        <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>18</v>
+        <v>5</v>
       </c>
       <c r="E13" s="3">
         <v>1005151</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="4">
         <v>40858</v>
       </c>
       <c r="G13" s="2"/>
@@ -730,15 +787,15 @@
         <v>37</v>
       </c>
       <c r="C14" t="s">
-        <v>10</v>
+        <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="E14" s="3">
         <v>1005151</v>
       </c>
-      <c r="F14" s="2">
+      <c r="F14" s="4">
         <v>38135</v>
       </c>
       <c r="G14" s="2"/>
@@ -751,15 +808,15 @@
         <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>17</v>
+        <v>4</v>
       </c>
       <c r="E15" s="3">
         <v>1005151</v>
       </c>
-      <c r="F15" s="2">
+      <c r="F15" s="4">
         <v>41356</v>
       </c>
       <c r="G15" s="2"/>
@@ -772,18 +829,333 @@
         <v>50</v>
       </c>
       <c r="C16" t="s">
+        <v>25</v>
+      </c>
+      <c r="D16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="3">
+        <v>1005151</v>
+      </c>
+      <c r="F16" s="4">
+        <v>38564</v>
+      </c>
+      <c r="G16" s="2"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f>A16+1</f>
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>45</v>
+      </c>
+      <c r="C17" t="s">
+        <v>26</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E17" s="3">
+        <v>2117272</v>
+      </c>
+      <c r="F17" s="4">
+        <v>42948</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" ref="A18:A30" si="0">A17+1</f>
         <v>17</v>
       </c>
-      <c r="E16" s="3">
-        <v>1005151</v>
-      </c>
-      <c r="F16" s="2">
-        <v>38564</v>
-      </c>
-      <c r="G16" s="2"/>
+      <c r="B18">
+        <v>92</v>
+      </c>
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" t="s">
+        <v>0</v>
+      </c>
+      <c r="E18" s="3">
+        <v>2117272</v>
+      </c>
+      <c r="F18" s="4">
+        <v>42948</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>34</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19" s="3">
+        <v>2117272</v>
+      </c>
+      <c r="F19" s="4">
+        <v>42960</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>54</v>
+      </c>
+      <c r="C20" t="s">
+        <v>29</v>
+      </c>
+      <c r="D20" t="s">
+        <v>2</v>
+      </c>
+      <c r="E20" s="3">
+        <v>2117272</v>
+      </c>
+      <c r="F20" s="4">
+        <v>42960</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>65</v>
+      </c>
+      <c r="C21" t="s">
+        <v>30</v>
+      </c>
+      <c r="D21" t="s">
+        <v>2</v>
+      </c>
+      <c r="E21" s="3">
+        <v>2117272</v>
+      </c>
+      <c r="F21" s="4">
+        <v>42980</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>85</v>
+      </c>
+      <c r="C22" t="s">
+        <v>31</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="3">
+        <v>2117272</v>
+      </c>
+      <c r="F22" s="4">
+        <v>43024</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>23</v>
+      </c>
+      <c r="C23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="3">
+        <v>2117272</v>
+      </c>
+      <c r="F23" s="4">
+        <v>43319</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24">
+        <v>42</v>
+      </c>
+      <c r="C24" t="s">
+        <v>33</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" s="3">
+        <v>2117272</v>
+      </c>
+      <c r="F24" s="4">
+        <v>42955</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25">
+        <v>55</v>
+      </c>
+      <c r="C25" t="s">
+        <v>34</v>
+      </c>
+      <c r="D25" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="3">
+        <v>2117272</v>
+      </c>
+      <c r="F25" s="4">
+        <v>43686</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26">
+        <v>43</v>
+      </c>
+      <c r="C26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D26" t="s">
+        <v>3</v>
+      </c>
+      <c r="E26" s="3">
+        <v>2117272</v>
+      </c>
+      <c r="F26" s="4">
+        <v>42957</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27">
+        <v>22</v>
+      </c>
+      <c r="C27" t="s">
+        <v>36</v>
+      </c>
+      <c r="D27" t="s">
+        <v>3</v>
+      </c>
+      <c r="E27" s="3">
+        <v>2117272</v>
+      </c>
+      <c r="F27" s="4">
+        <v>42958</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28">
+        <v>21</v>
+      </c>
+      <c r="C28" t="s">
+        <v>37</v>
+      </c>
+      <c r="D28" t="s">
+        <v>5</v>
+      </c>
+      <c r="E28" s="3">
+        <v>2117272</v>
+      </c>
+      <c r="F28" s="4">
+        <v>43842</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29">
+        <v>19</v>
+      </c>
+      <c r="C29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D29" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="3">
+        <v>2117272</v>
+      </c>
+      <c r="F29" s="4">
+        <v>42960</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30">
+        <v>23</v>
+      </c>
+      <c r="C30" t="s">
+        <v>39</v>
+      </c>
+      <c r="D30" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="3">
+        <v>2117272</v>
+      </c>
+      <c r="F30" s="4">
+        <v>42961</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f>A30+1</f>
+        <v>30</v>
+      </c>
+      <c r="B31">
+        <v>40</v>
+      </c>
+      <c r="C31" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" t="s">
+        <v>4</v>
+      </c>
+      <c r="E31" s="3">
+        <v>2117272</v>
+      </c>
+      <c r="F31" s="4">
+        <v>42962</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>